<commit_message>
Version 2.0 (finished, working)
Comments adjusted and unsuitable if conditions fixed.
</commit_message>
<xml_diff>
--- a/alltoys.xlsx
+++ b/alltoys.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PyCharm\region_founder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PyCharm\Projects\region_founder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9575D1C-25BF-4B32-86DC-9BE4CCDC5CB7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906853E3-E9BF-48E5-9047-52EE48E3CD6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>35</v>
       </c>
       <c r="C25" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>27</v>
       </c>
       <c r="C35" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>28</v>
       </c>
       <c r="C36" s="2">
-        <v>42714.330988922164</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>